<commit_message>
WIP: modified main file (LR for real fathers)
</commit_message>
<xml_diff>
--- a/ASTR_AVAR.xlsx
+++ b/ASTR_AVAR.xlsx
@@ -139,10 +139,10 @@
     <t xml:space="preserve">D8S1132_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Penta D_1</t>
+    <t xml:space="preserve">Penta-D_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Penta D_2</t>
+    <t xml:space="preserve">Penta-D_2</t>
   </si>
   <si>
     <t xml:space="preserve">D21S2050_1</t>
@@ -157,10 +157,10 @@
     <t xml:space="preserve">D7S1517_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Penta E_1</t>
+    <t xml:space="preserve">Penta-E_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Penta E_2</t>
+    <t xml:space="preserve">Penta-E_2</t>
   </si>
   <si>
     <t xml:space="preserve">D3S1358_1</t>
@@ -382,7 +382,7 @@
     <t xml:space="preserve">15.2</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_12</t>
+    <t xml:space="preserve">ShR_12</t>
   </si>
   <si>
     <t xml:space="preserve">20.1</t>
@@ -397,7 +397,7 @@
     <t xml:space="preserve">27.2</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_13</t>
+    <t xml:space="preserve">ShR_13</t>
   </si>
   <si>
     <t xml:space="preserve">23.2</t>
@@ -409,7 +409,7 @@
     <t xml:space="preserve">17.3</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_19</t>
+    <t xml:space="preserve">ShR_19</t>
   </si>
   <si>
     <t xml:space="preserve">19.1</t>
@@ -424,7 +424,7 @@
     <t xml:space="preserve">24.2</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_20</t>
+    <t xml:space="preserve">ShR_20</t>
   </si>
   <si>
     <t xml:space="preserve">34</t>
@@ -433,7 +433,7 @@
     <t xml:space="preserve">20.2</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_22</t>
+    <t xml:space="preserve">ShR_22</t>
   </si>
   <si>
     <t xml:space="preserve">35</t>
@@ -442,25 +442,25 @@
     <t xml:space="preserve">30</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_23</t>
+    <t xml:space="preserve">ShR_23</t>
   </si>
   <si>
     <t xml:space="preserve">9.3</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_25</t>
+    <t xml:space="preserve">ShR_25</t>
   </si>
   <si>
     <t xml:space="preserve">29.2</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_26</t>
+    <t xml:space="preserve">ShR_26</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_27</t>
+    <t xml:space="preserve">ShR_27</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_29</t>
+    <t xml:space="preserve">ShR_29</t>
   </si>
   <si>
     <t xml:space="preserve">18.3</t>
@@ -469,49 +469,49 @@
     <t xml:space="preserve">22.2</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_30</t>
+    <t xml:space="preserve">ShR_30</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_31</t>
+    <t xml:space="preserve">ShR_31</t>
   </si>
   <si>
     <t xml:space="preserve">18.1</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_32</t>
+    <t xml:space="preserve">ShR_32</t>
   </si>
   <si>
     <t xml:space="preserve">16.3</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_34</t>
+    <t xml:space="preserve">ShR_34</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_48</t>
+    <t xml:space="preserve">ShR_48</t>
   </si>
   <si>
     <t xml:space="preserve">32</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_5</t>
+    <t xml:space="preserve">ShR_5</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_51</t>
+    <t xml:space="preserve">ShR_51</t>
   </si>
   <si>
     <t xml:space="preserve">36</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_57</t>
+    <t xml:space="preserve">ShR_57</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_58</t>
+    <t xml:space="preserve">ShR_58</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_59</t>
+    <t xml:space="preserve">ShR_59</t>
   </si>
   <si>
-    <t xml:space="preserve"> ShR_6</t>
+    <t xml:space="preserve">ShR_6</t>
   </si>
   <si>
     <t xml:space="preserve">DGU</t>
@@ -1294,14 +1294,14 @@
   </sheetPr>
   <dimension ref="A1:CK190"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BC18" activeCellId="0" sqref="BC18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AU6" activeCellId="0" sqref="AU6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="48" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="6.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="60" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="1" width="12.86"/>

</xml_diff>